<commit_message>
Started Doing DSA Sheet
</commit_message>
<xml_diff>
--- a/Java Practice/Love Babbar DSA Questions/FINAL450.xlsx
+++ b/Java Practice/Love Babbar DSA Questions/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Practice\Java Practice\Love Babbar DSA Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDD28FC-8665-4459-BC3B-A9E1445AB182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18490D48-F2F6-4952-89D5-B0BEF88994F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,6 +1426,12 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
+  </si>
+  <si>
+    <t>O(n) left</t>
+  </si>
+  <si>
+    <t>one solution left</t>
   </si>
 </sst>
 </file>
@@ -1495,7 +1501,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1514,6 +1520,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1528,7 +1540,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1553,6 +1565,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1870,10 +1885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:C481"/>
+  <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1883,17 +1898,17 @@
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25">
+    <row r="1" spans="1:4" ht="25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="B2" s="9" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21">
+    <row r="4" spans="1:4" ht="21">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1904,12 +1919,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21">
+    <row r="6" spans="1:4" ht="21">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1920,7 +1935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21">
+    <row r="7" spans="1:4" ht="21">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1931,40 +1946,46 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21">
+    <row r="8" spans="1:4" ht="21">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="21">
+      <c r="C8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="21">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="21">
+      <c r="C9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="21">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="21">
+      <c r="C10" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="21">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -1975,7 +1996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21">
+    <row r="12" spans="1:4" ht="21">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -1986,7 +2007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21">
+    <row r="13" spans="1:4" ht="21">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -1997,7 +2018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21">
+    <row r="14" spans="1:4" ht="21">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -2008,7 +2029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21">
+    <row r="15" spans="1:4" ht="21">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
@@ -2019,7 +2040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="21">
+    <row r="16" spans="1:4" ht="21">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Started Level up course by Prateek Bhaiya
</commit_message>
<xml_diff>
--- a/Java Practice/Love Babbar DSA Questions/FINAL450.xlsx
+++ b/Java Practice/Love Babbar DSA Questions/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Practice\Java Practice\Love Babbar DSA Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18490D48-F2F6-4952-89D5-B0BEF88994F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D5EFCF-0B59-444D-893E-DD75EF3C7940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1501,7 +1501,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1526,6 +1526,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1540,7 +1546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1568,6 +1574,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1887,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1992,7 +2001,7 @@
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2003,7 +2012,7 @@
       <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2014,7 +2023,7 @@
       <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2025,7 +2034,7 @@
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2036,7 +2045,7 @@
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2047,7 +2056,7 @@
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="13" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>